<commit_message>
Started working on tranmission between comp and FPGAs
</commit_message>
<xml_diff>
--- a/wallace_tree_fixed_2.xlsx
+++ b/wallace_tree_fixed_2.xlsx
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:AMJ70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK85" activeCellId="0" sqref="AK85"/>
+      <selection pane="topLeft" activeCell="G74" activeCellId="0" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6742,7 +6742,7 @@
       <c r="U64" s="50"/>
       <c r="V64" s="50"/>
       <c r="W64" s="50" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X64" s="50"/>
       <c r="Y64" s="50"/>
@@ -7043,6 +7043,7 @@
       <c r="AX69" s="124"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G70" s="34"/>
       <c r="H70" s="34"/>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>

</xml_diff>